<commit_message>
Updated Ghatt and added on click to edit and delete
</commit_message>
<xml_diff>
--- a/Gantt_Chart_Group30.xlsx
+++ b/Gantt_Chart_Group30.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenri\Documents\GitHub\COP4331C-ContactManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF2005B-895A-425A-B243-DF68647C5C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16944463-5D80-4BC7-8ACA-0E7B8B92D4A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
   <si>
     <t>Project Start:</t>
   </si>
@@ -194,9 +194,6 @@
     <t>Login and Registration</t>
   </si>
   <si>
-    <t>Contact Editing</t>
-  </si>
-  <si>
     <t>ContactCircuit</t>
   </si>
   <si>
@@ -230,9 +227,6 @@
     <t>Goal Deadline</t>
   </si>
   <si>
-    <t>Not Complete</t>
-  </si>
-  <si>
     <t>Presentation Date</t>
   </si>
   <si>
@@ -243,6 +237,12 @@
   </si>
   <si>
     <t>Floyd</t>
+  </si>
+  <si>
+    <t>Fabian+Maya</t>
+  </si>
+  <si>
+    <t>Contact Srch/+/-/Edit</t>
   </si>
 </sst>
 </file>
@@ -949,6 +949,12 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -965,12 +971,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1532,8 +1532,8 @@
   <dimension ref="A1:BE36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC19" sqref="AC19"/>
+      <pane ySplit="6" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1552,7 +1552,7 @@
   <sheetData>
     <row r="1" spans="1:57" ht="28.5" x14ac:dyDescent="0.65">
       <c r="B1" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1560,49 +1560,49 @@
       <c r="F1" s="78"/>
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="86"/>
-      <c r="O1" s="86"/>
-      <c r="P1" s="86"/>
-      <c r="Q1" s="86"/>
-      <c r="R1" s="86"/>
-      <c r="S1" s="86"/>
-      <c r="T1" s="86"/>
-      <c r="U1" s="86"/>
-      <c r="V1" s="86"/>
-      <c r="W1" s="86"/>
-      <c r="X1" s="86"/>
-      <c r="Y1" s="86"/>
-      <c r="Z1" s="86"/>
-      <c r="AA1" s="86"/>
+      <c r="J1" s="88"/>
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="88"/>
+      <c r="O1" s="88"/>
+      <c r="P1" s="88"/>
+      <c r="Q1" s="88"/>
+      <c r="R1" s="88"/>
+      <c r="S1" s="88"/>
+      <c r="T1" s="88"/>
+      <c r="U1" s="88"/>
+      <c r="V1" s="88"/>
+      <c r="W1" s="88"/>
+      <c r="X1" s="88"/>
+      <c r="Y1" s="88"/>
+      <c r="Z1" s="88"/>
+      <c r="AA1" s="88"/>
     </row>
     <row r="2" spans="1:57" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="90">
+      <c r="E2" s="92">
         <v>45663</v>
       </c>
-      <c r="F2" s="91"/>
+      <c r="F2" s="93"/>
     </row>
     <row r="3" spans="1:57" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="90">
+      <c r="E3" s="92">
         <f ca="1">TODAY()</f>
-        <v>45684</v>
-      </c>
-      <c r="F3" s="91"/>
+        <v>45686</v>
+      </c>
+      <c r="F3" s="93"/>
     </row>
     <row r="4" spans="1:57" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D4" s="6" t="s">
@@ -1611,76 +1611,76 @@
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="87">
+      <c r="I4" s="89">
         <f>I5</f>
         <v>45663</v>
       </c>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="89"/>
-      <c r="P4" s="87">
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="91"/>
+      <c r="P4" s="89">
         <f>P5</f>
         <v>45670</v>
       </c>
-      <c r="Q4" s="88"/>
-      <c r="R4" s="88"/>
-      <c r="S4" s="88"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="88"/>
-      <c r="V4" s="89"/>
-      <c r="W4" s="87">
+      <c r="Q4" s="90"/>
+      <c r="R4" s="90"/>
+      <c r="S4" s="90"/>
+      <c r="T4" s="90"/>
+      <c r="U4" s="90"/>
+      <c r="V4" s="91"/>
+      <c r="W4" s="89">
         <f>W5</f>
         <v>45677</v>
       </c>
-      <c r="X4" s="88"/>
-      <c r="Y4" s="88"/>
-      <c r="Z4" s="88"/>
-      <c r="AA4" s="88"/>
-      <c r="AB4" s="88"/>
-      <c r="AC4" s="89"/>
-      <c r="AD4" s="87">
+      <c r="X4" s="90"/>
+      <c r="Y4" s="90"/>
+      <c r="Z4" s="90"/>
+      <c r="AA4" s="90"/>
+      <c r="AB4" s="90"/>
+      <c r="AC4" s="91"/>
+      <c r="AD4" s="89">
         <f>AD5</f>
         <v>45684</v>
       </c>
-      <c r="AE4" s="88"/>
-      <c r="AF4" s="88"/>
-      <c r="AG4" s="88"/>
-      <c r="AH4" s="88"/>
-      <c r="AI4" s="88"/>
-      <c r="AJ4" s="89"/>
-      <c r="AK4" s="87">
+      <c r="AE4" s="90"/>
+      <c r="AF4" s="90"/>
+      <c r="AG4" s="90"/>
+      <c r="AH4" s="90"/>
+      <c r="AI4" s="90"/>
+      <c r="AJ4" s="91"/>
+      <c r="AK4" s="89">
         <f>AK5</f>
         <v>45691</v>
       </c>
-      <c r="AL4" s="88"/>
-      <c r="AM4" s="88"/>
-      <c r="AN4" s="88"/>
-      <c r="AO4" s="88"/>
-      <c r="AP4" s="88"/>
-      <c r="AQ4" s="89"/>
-      <c r="AR4" s="87">
+      <c r="AL4" s="90"/>
+      <c r="AM4" s="90"/>
+      <c r="AN4" s="90"/>
+      <c r="AO4" s="90"/>
+      <c r="AP4" s="90"/>
+      <c r="AQ4" s="91"/>
+      <c r="AR4" s="89">
         <f>AR5</f>
         <v>45698</v>
       </c>
-      <c r="AS4" s="88"/>
-      <c r="AT4" s="88"/>
-      <c r="AU4" s="88"/>
-      <c r="AV4" s="88"/>
-      <c r="AW4" s="88"/>
-      <c r="AX4" s="89"/>
-      <c r="AY4" s="87">
+      <c r="AS4" s="90"/>
+      <c r="AT4" s="90"/>
+      <c r="AU4" s="90"/>
+      <c r="AV4" s="90"/>
+      <c r="AW4" s="90"/>
+      <c r="AX4" s="91"/>
+      <c r="AY4" s="89">
         <f>AY5</f>
         <v>45705</v>
       </c>
-      <c r="AZ4" s="88"/>
-      <c r="BA4" s="88"/>
-      <c r="BB4" s="88"/>
-      <c r="BC4" s="88"/>
-      <c r="BD4" s="88"/>
-      <c r="BE4" s="89"/>
+      <c r="AZ4" s="90"/>
+      <c r="BA4" s="90"/>
+      <c r="BB4" s="90"/>
+      <c r="BC4" s="90"/>
+      <c r="BD4" s="90"/>
+      <c r="BE4" s="91"/>
     </row>
     <row r="5" spans="1:57" x14ac:dyDescent="0.35">
       <c r="A5" s="6"/>
@@ -2103,14 +2103,14 @@
     <row r="7" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="19"/>
       <c r="B7" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="21"/>
       <c r="D7" s="22"/>
-      <c r="E7" s="93">
+      <c r="E7" s="87">
         <v>45704</v>
       </c>
-      <c r="F7" s="93"/>
+      <c r="F7" s="87"/>
       <c r="G7" s="23"/>
       <c r="H7" s="23" t="str">
         <f t="shared" ref="H7:H32" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
@@ -2169,14 +2169,14 @@
     <row r="8" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="19"/>
       <c r="B8" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="21"/>
       <c r="D8" s="22"/>
-      <c r="E8" s="93">
+      <c r="E8" s="87">
         <v>45697</v>
       </c>
-      <c r="F8" s="93"/>
+      <c r="F8" s="87"/>
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
       <c r="I8" s="64"/>
@@ -2232,7 +2232,7 @@
     <row r="9" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="19"/>
       <c r="B9" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="26"/>
@@ -2438,7 +2438,7 @@
     <row r="12" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="19"/>
       <c r="B12" s="29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="30"/>
       <c r="D12" s="31">
@@ -2508,7 +2508,7 @@
         <v>29</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D13" s="31">
         <v>0</v>
@@ -2577,14 +2577,14 @@
     <row r="14" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="19"/>
       <c r="B14" s="29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C14" s="30"/>
       <c r="D14" s="31"/>
-      <c r="E14" s="92" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="92"/>
+      <c r="E14" s="86" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="86"/>
       <c r="G14" s="23"/>
       <c r="H14" s="23"/>
       <c r="I14" s="64"/>
@@ -2928,10 +2928,10 @@
       <c r="D19" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="92">
+      <c r="E19" s="86">
         <v>45671</v>
       </c>
-      <c r="F19" s="92"/>
+      <c r="F19" s="86"/>
       <c r="G19" s="23"/>
       <c r="H19" s="23" t="str">
         <f t="shared" si="5"/>
@@ -3060,7 +3060,7 @@
         <v>35</v>
       </c>
       <c r="D21" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="32">
         <v>45667</v>
@@ -3126,13 +3126,13 @@
     <row r="22" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="19"/>
       <c r="B22" s="47" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C22" s="48" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D22" s="49">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="E22" s="32">
         <v>45667</v>
@@ -3198,13 +3198,13 @@
     <row r="23" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="19"/>
       <c r="B23" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" s="48" t="s">
         <v>35</v>
       </c>
       <c r="D23" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="32">
         <v>45677</v>
@@ -3270,11 +3270,11 @@
     <row r="24" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="19"/>
       <c r="B24" s="47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" s="48"/>
       <c r="D24" s="49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E24" s="32">
         <v>45667</v>
@@ -3343,15 +3343,15 @@
         <v>30</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D25" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="92">
+      <c r="E25" s="86">
         <v>45678</v>
       </c>
-      <c r="F25" s="92"/>
+      <c r="F25" s="86"/>
       <c r="G25" s="23"/>
       <c r="H25" s="23" t="str">
         <f t="shared" si="5"/>
@@ -3544,10 +3544,10 @@
     <row r="28" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="19"/>
       <c r="B28" s="55" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" s="56" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D28" s="57">
         <v>0</v>
@@ -3616,7 +3616,7 @@
     <row r="29" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="19"/>
       <c r="B29" s="55" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29" s="56"/>
       <c r="D29" s="57">
@@ -3686,7 +3686,7 @@
     <row r="30" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="19"/>
       <c r="B30" s="55" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C30" s="56"/>
       <c r="D30" s="57">
@@ -3758,14 +3758,16 @@
       <c r="B31" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="56"/>
+      <c r="C31" s="56" t="s">
+        <v>53</v>
+      </c>
       <c r="D31" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="E31" s="92">
+        <v>34</v>
+      </c>
+      <c r="E31" s="86">
         <v>45685</v>
       </c>
-      <c r="F31" s="92"/>
+      <c r="F31" s="86"/>
       <c r="G31" s="23"/>
       <c r="H31" s="23" t="str">
         <f t="shared" si="5"/>
@@ -3903,12 +3905,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E14:F14"/>
     <mergeCell ref="J1:AA1"/>
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
@@ -3919,6 +3915,12 @@
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E14:F14"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D32">
     <cfRule type="dataBar" priority="12">

</xml_diff>

<commit_message>
Added edit/delet icons, fixed register password verification, 'No contacts searched', Fixed Search button and Create Contact button, Updated About Us pictures, Fixed mobile view
</commit_message>
<xml_diff>
--- a/Gantt_Chart_Group30.xlsx
+++ b/Gantt_Chart_Group30.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenri\Documents\GitHub\COP4331C-ContactManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayal\OneDrive\Desktop\COP4331C-ContactManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16944463-5D80-4BC7-8ACA-0E7B8B92D4A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F521C2E1-61A3-420D-BF6E-4B4A419C45DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10365" yWindow="4755" windowWidth="21660" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
     <sheet name="About" sheetId="12" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">ProjectSchedule!$1:$32</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">ProjectSchedule!$1:$33</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">ProjectSchedule!$4:$6</definedName>
     <definedName name="task_end" localSheetId="0">ProjectSchedule!$F1</definedName>
     <definedName name="task_progress" localSheetId="0">ProjectSchedule!$D1</definedName>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
   <si>
     <t>Project Start:</t>
   </si>
@@ -221,9 +221,6 @@
     <t>Framework</t>
   </si>
   <si>
-    <t>Implement Design</t>
-  </si>
-  <si>
     <t>Goal Deadline</t>
   </si>
   <si>
@@ -239,10 +236,19 @@
     <t>Floyd</t>
   </si>
   <si>
-    <t>Fabian+Maya</t>
-  </si>
-  <si>
     <t>Contact Srch/+/-/Edit</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Accessibility</t>
+  </si>
+  <si>
+    <t>Maya</t>
+  </si>
+  <si>
+    <t>Fabian/Maya</t>
   </si>
 </sst>
 </file>
@@ -949,28 +955,28 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1529,28 +1535,28 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BE36"/>
+  <dimension ref="A1:BE37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X25" sqref="X25"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" customWidth="1"/>
-    <col min="2" max="2" width="29.08984375" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.453125" customWidth="1"/>
-    <col min="7" max="7" width="2.81640625" customWidth="1"/>
-    <col min="8" max="8" width="6.1796875" hidden="1" customWidth="1"/>
-    <col min="9" max="57" width="2.54296875" customWidth="1"/>
-    <col min="62" max="63" width="10.1796875"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="2.85546875" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" hidden="1" customWidth="1"/>
+    <col min="9" max="57" width="2.5703125" customWidth="1"/>
+    <col min="62" max="63" width="10.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:57" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B1" s="16" t="s">
         <v>38</v>
       </c>
@@ -1560,129 +1566,129 @@
       <c r="F1" s="78"/>
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="88"/>
-      <c r="O1" s="88"/>
-      <c r="P1" s="88"/>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="88"/>
-      <c r="S1" s="88"/>
-      <c r="T1" s="88"/>
-      <c r="U1" s="88"/>
-      <c r="V1" s="88"/>
-      <c r="W1" s="88"/>
-      <c r="X1" s="88"/>
-      <c r="Y1" s="88"/>
-      <c r="Z1" s="88"/>
-      <c r="AA1" s="88"/>
-    </row>
-    <row r="2" spans="1:57" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="86"/>
+      <c r="O1" s="86"/>
+      <c r="P1" s="86"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="86"/>
+      <c r="S1" s="86"/>
+      <c r="T1" s="86"/>
+      <c r="U1" s="86"/>
+      <c r="V1" s="86"/>
+      <c r="W1" s="86"/>
+      <c r="X1" s="86"/>
+      <c r="Y1" s="86"/>
+      <c r="Z1" s="86"/>
+      <c r="AA1" s="86"/>
+    </row>
+    <row r="2" spans="1:57" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
         <v>39</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="92">
+      <c r="E2" s="90">
         <v>45663</v>
       </c>
-      <c r="F2" s="93"/>
-    </row>
-    <row r="3" spans="1:57" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F2" s="91"/>
+    </row>
+    <row r="3" spans="1:57" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="92">
+      <c r="E3" s="90">
         <f ca="1">TODAY()</f>
-        <v>45686</v>
-      </c>
-      <c r="F3" s="93"/>
-    </row>
-    <row r="4" spans="1:57" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>45691</v>
+      </c>
+      <c r="F3" s="91"/>
+    </row>
+    <row r="4" spans="1:57" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="89">
+      <c r="I4" s="87">
         <f>I5</f>
         <v>45663</v>
       </c>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
-      <c r="O4" s="91"/>
-      <c r="P4" s="89">
+      <c r="J4" s="88"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88"/>
+      <c r="M4" s="88"/>
+      <c r="N4" s="88"/>
+      <c r="O4" s="89"/>
+      <c r="P4" s="87">
         <f>P5</f>
         <v>45670</v>
       </c>
-      <c r="Q4" s="90"/>
-      <c r="R4" s="90"/>
-      <c r="S4" s="90"/>
-      <c r="T4" s="90"/>
-      <c r="U4" s="90"/>
-      <c r="V4" s="91"/>
-      <c r="W4" s="89">
+      <c r="Q4" s="88"/>
+      <c r="R4" s="88"/>
+      <c r="S4" s="88"/>
+      <c r="T4" s="88"/>
+      <c r="U4" s="88"/>
+      <c r="V4" s="89"/>
+      <c r="W4" s="87">
         <f>W5</f>
         <v>45677</v>
       </c>
-      <c r="X4" s="90"/>
-      <c r="Y4" s="90"/>
-      <c r="Z4" s="90"/>
-      <c r="AA4" s="90"/>
-      <c r="AB4" s="90"/>
-      <c r="AC4" s="91"/>
-      <c r="AD4" s="89">
+      <c r="X4" s="88"/>
+      <c r="Y4" s="88"/>
+      <c r="Z4" s="88"/>
+      <c r="AA4" s="88"/>
+      <c r="AB4" s="88"/>
+      <c r="AC4" s="89"/>
+      <c r="AD4" s="87">
         <f>AD5</f>
         <v>45684</v>
       </c>
-      <c r="AE4" s="90"/>
-      <c r="AF4" s="90"/>
-      <c r="AG4" s="90"/>
-      <c r="AH4" s="90"/>
-      <c r="AI4" s="90"/>
-      <c r="AJ4" s="91"/>
-      <c r="AK4" s="89">
+      <c r="AE4" s="88"/>
+      <c r="AF4" s="88"/>
+      <c r="AG4" s="88"/>
+      <c r="AH4" s="88"/>
+      <c r="AI4" s="88"/>
+      <c r="AJ4" s="89"/>
+      <c r="AK4" s="87">
         <f>AK5</f>
         <v>45691</v>
       </c>
-      <c r="AL4" s="90"/>
-      <c r="AM4" s="90"/>
-      <c r="AN4" s="90"/>
-      <c r="AO4" s="90"/>
-      <c r="AP4" s="90"/>
-      <c r="AQ4" s="91"/>
-      <c r="AR4" s="89">
+      <c r="AL4" s="88"/>
+      <c r="AM4" s="88"/>
+      <c r="AN4" s="88"/>
+      <c r="AO4" s="88"/>
+      <c r="AP4" s="88"/>
+      <c r="AQ4" s="89"/>
+      <c r="AR4" s="87">
         <f>AR5</f>
         <v>45698</v>
       </c>
-      <c r="AS4" s="90"/>
-      <c r="AT4" s="90"/>
-      <c r="AU4" s="90"/>
-      <c r="AV4" s="90"/>
-      <c r="AW4" s="90"/>
-      <c r="AX4" s="91"/>
-      <c r="AY4" s="89">
+      <c r="AS4" s="88"/>
+      <c r="AT4" s="88"/>
+      <c r="AU4" s="88"/>
+      <c r="AV4" s="88"/>
+      <c r="AW4" s="88"/>
+      <c r="AX4" s="89"/>
+      <c r="AY4" s="87">
         <f>AY5</f>
         <v>45705</v>
       </c>
-      <c r="AZ4" s="90"/>
-      <c r="BA4" s="90"/>
-      <c r="BB4" s="90"/>
-      <c r="BC4" s="90"/>
-      <c r="BD4" s="90"/>
-      <c r="BE4" s="91"/>
-    </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.35">
+      <c r="AZ4" s="88"/>
+      <c r="BA4" s="88"/>
+      <c r="BB4" s="88"/>
+      <c r="BC4" s="88"/>
+      <c r="BD4" s="88"/>
+      <c r="BE4" s="89"/>
+    </row>
+    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="G5" s="6"/>
       <c r="I5" s="13">
@@ -1882,7 +1888,7 @@
         <v>45711</v>
       </c>
     </row>
-    <row r="6" spans="1:57" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:57" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
       <c r="B6" s="10" t="s">
         <v>8</v>
@@ -2100,20 +2106,20 @@
         <v>S</v>
       </c>
     </row>
-    <row r="7" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19"/>
       <c r="B7" s="20" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="21"/>
       <c r="D7" s="22"/>
-      <c r="E7" s="87">
+      <c r="E7" s="93">
         <v>45704</v>
       </c>
-      <c r="F7" s="87"/>
+      <c r="F7" s="93"/>
       <c r="G7" s="23"/>
       <c r="H7" s="23" t="str">
-        <f t="shared" ref="H7:H32" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H7:H33" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I7" s="64"/>
@@ -2166,17 +2172,17 @@
       <c r="BD7" s="64"/>
       <c r="BE7" s="64"/>
     </row>
-    <row r="8" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19"/>
       <c r="B8" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="21"/>
       <c r="D8" s="22"/>
-      <c r="E8" s="87">
+      <c r="E8" s="93">
         <v>45697</v>
       </c>
-      <c r="F8" s="87"/>
+      <c r="F8" s="93"/>
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
       <c r="I8" s="64"/>
@@ -2229,7 +2235,7 @@
       <c r="BD8" s="64"/>
       <c r="BE8" s="64"/>
     </row>
-    <row r="9" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19"/>
       <c r="B9" s="24" t="s">
         <v>44</v>
@@ -2293,7 +2299,7 @@
       <c r="BD9" s="64"/>
       <c r="BE9" s="64"/>
     </row>
-    <row r="10" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19"/>
       <c r="B10" s="29" t="s">
         <v>26</v>
@@ -2365,7 +2371,7 @@
       <c r="BD10" s="64"/>
       <c r="BE10" s="64"/>
     </row>
-    <row r="11" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19"/>
       <c r="B11" s="29" t="s">
         <v>28</v>
@@ -2435,7 +2441,7 @@
       <c r="BD11" s="64"/>
       <c r="BE11" s="64"/>
     </row>
-    <row r="12" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19"/>
       <c r="B12" s="29" t="s">
         <v>43</v>
@@ -2502,13 +2508,13 @@
       <c r="BD12" s="64"/>
       <c r="BE12" s="64"/>
     </row>
-    <row r="13" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
       <c r="B13" s="29" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D13" s="31">
         <v>0</v>
@@ -2574,17 +2580,17 @@
       <c r="BD13" s="64"/>
       <c r="BE13" s="64"/>
     </row>
-    <row r="14" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19"/>
       <c r="B14" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" s="30"/>
       <c r="D14" s="31"/>
-      <c r="E14" s="86" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="86"/>
+      <c r="E14" s="92" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="92"/>
       <c r="G14" s="23"/>
       <c r="H14" s="23"/>
       <c r="I14" s="64"/>
@@ -2637,7 +2643,7 @@
       <c r="BD14" s="64"/>
       <c r="BE14" s="64"/>
     </row>
-    <row r="15" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19"/>
       <c r="B15" s="34" t="s">
         <v>23</v>
@@ -2701,7 +2707,7 @@
       <c r="BD15" s="64"/>
       <c r="BE15" s="64"/>
     </row>
-    <row r="16" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19"/>
       <c r="B16" s="39" t="s">
         <v>32</v>
@@ -2773,7 +2779,7 @@
       <c r="BD16" s="64"/>
       <c r="BE16" s="64"/>
     </row>
-    <row r="17" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19"/>
       <c r="B17" s="39" t="s">
         <v>33</v>
@@ -2845,7 +2851,7 @@
       <c r="BD17" s="64"/>
       <c r="BE17" s="64"/>
     </row>
-    <row r="18" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19"/>
       <c r="B18" s="39" t="s">
         <v>31</v>
@@ -2917,7 +2923,7 @@
       <c r="BD18" s="64"/>
       <c r="BE18" s="64"/>
     </row>
-    <row r="19" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19"/>
       <c r="B19" s="39" t="s">
         <v>30</v>
@@ -2928,10 +2934,10 @@
       <c r="D19" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="86">
+      <c r="E19" s="92">
         <v>45671</v>
       </c>
-      <c r="F19" s="86"/>
+      <c r="F19" s="92"/>
       <c r="G19" s="23"/>
       <c r="H19" s="23" t="str">
         <f t="shared" si="5"/>
@@ -2987,7 +2993,7 @@
       <c r="BD19" s="64"/>
       <c r="BE19" s="64"/>
     </row>
-    <row r="20" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="19"/>
       <c r="B20" s="42" t="s">
         <v>24</v>
@@ -3051,7 +3057,7 @@
       <c r="BD20" s="64"/>
       <c r="BE20" s="64"/>
     </row>
-    <row r="21" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
       <c r="B21" s="47" t="s">
         <v>37</v>
@@ -3123,13 +3129,13 @@
       <c r="BD21" s="64"/>
       <c r="BE21" s="64"/>
     </row>
-    <row r="22" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="19"/>
       <c r="B22" s="47" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C22" s="48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D22" s="49">
         <v>0.75</v>
@@ -3195,7 +3201,7 @@
       <c r="BD22" s="64"/>
       <c r="BE22" s="64"/>
     </row>
-    <row r="23" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
       <c r="B23" s="47" t="s">
         <v>42</v>
@@ -3267,7 +3273,7 @@
       <c r="BD23" s="64"/>
       <c r="BE23" s="64"/>
     </row>
-    <row r="24" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="19"/>
       <c r="B24" s="47" t="s">
         <v>45</v>
@@ -3337,21 +3343,21 @@
       <c r="BD24" s="64"/>
       <c r="BE24" s="64"/>
     </row>
-    <row r="25" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="47" t="s">
         <v>30</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D25" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="86">
+      <c r="E25" s="92">
         <v>45678</v>
       </c>
-      <c r="F25" s="86"/>
+      <c r="F25" s="92"/>
       <c r="G25" s="23"/>
       <c r="H25" s="23" t="str">
         <f t="shared" si="5"/>
@@ -3407,7 +3413,7 @@
       <c r="BD25" s="64"/>
       <c r="BE25" s="64"/>
     </row>
-    <row r="26" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="50" t="s">
         <v>25</v>
@@ -3471,12 +3477,14 @@
       <c r="BD26" s="64"/>
       <c r="BE26" s="64"/>
     </row>
-    <row r="27" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
       <c r="B27" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="56"/>
+      <c r="C27" s="56" t="s">
+        <v>35</v>
+      </c>
       <c r="D27" s="57">
         <v>1</v>
       </c>
@@ -3484,12 +3492,12 @@
         <v>45665</v>
       </c>
       <c r="F27" s="33">
-        <v>45669</v>
+        <v>45665</v>
       </c>
       <c r="G27" s="23"/>
       <c r="H27" s="23">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I27" s="64"/>
       <c r="J27" s="64"/>
@@ -3541,16 +3549,16 @@
       <c r="BD27" s="64"/>
       <c r="BE27" s="64"/>
     </row>
-    <row r="28" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19"/>
       <c r="B28" s="55" t="s">
         <v>46</v>
       </c>
       <c r="C28" s="56" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D28" s="57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="32">
         <v>45672</v>
@@ -3613,14 +3621,16 @@
       <c r="BD28" s="64"/>
       <c r="BE28" s="64"/>
     </row>
-    <row r="29" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="19"/>
       <c r="B29" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="56"/>
+        <v>53</v>
+      </c>
+      <c r="C29" s="56" t="s">
+        <v>55</v>
+      </c>
       <c r="D29" s="57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="32">
         <v>45677</v>
@@ -3683,26 +3693,25 @@
       <c r="BD29" s="64"/>
       <c r="BE29" s="64"/>
     </row>
-    <row r="30" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="19"/>
       <c r="B30" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="56"/>
+        <v>54</v>
+      </c>
+      <c r="C30" s="56" t="s">
+        <v>55</v>
+      </c>
       <c r="D30" s="57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="32">
-        <v>45682</v>
+        <v>45684</v>
       </c>
       <c r="F30" s="33">
-        <v>45695</v>
+        <v>45690</v>
       </c>
       <c r="G30" s="23"/>
-      <c r="H30" s="23">
-        <f t="shared" si="5"/>
-        <v>14</v>
-      </c>
+      <c r="H30" s="23"/>
       <c r="I30" s="64"/>
       <c r="J30" s="64"/>
       <c r="K30" s="64"/>
@@ -3753,25 +3762,27 @@
       <c r="BD30" s="64"/>
       <c r="BE30" s="64"/>
     </row>
-    <row r="31" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="19"/>
       <c r="B31" s="55" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C31" s="56" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="57" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" s="86">
-        <v>45685</v>
-      </c>
-      <c r="F31" s="86"/>
+        <v>56</v>
+      </c>
+      <c r="D31" s="57">
+        <v>1</v>
+      </c>
+      <c r="E31" s="32">
+        <v>45682</v>
+      </c>
+      <c r="F31" s="33">
+        <v>45695</v>
+      </c>
       <c r="G31" s="23"/>
-      <c r="H31" s="23" t="str">
+      <c r="H31" s="23">
         <f t="shared" si="5"/>
-        <v/>
+        <v>14</v>
       </c>
       <c r="I31" s="64"/>
       <c r="J31" s="64"/>
@@ -3795,7 +3806,7 @@
       <c r="AB31" s="64"/>
       <c r="AC31" s="64"/>
       <c r="AD31" s="64"/>
-      <c r="AE31" s="83"/>
+      <c r="AE31" s="64"/>
       <c r="AF31" s="64"/>
       <c r="AG31" s="64"/>
       <c r="AH31" s="64"/>
@@ -3823,88 +3834,164 @@
       <c r="BD31" s="64"/>
       <c r="BE31" s="64"/>
     </row>
-    <row r="32" spans="1:57" s="3" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="19"/>
-      <c r="B32" s="58"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="62"/>
-      <c r="G32" s="63"/>
-      <c r="H32" s="63" t="str">
+      <c r="B32" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="92">
+        <v>45685</v>
+      </c>
+      <c r="F32" s="92"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="I32" s="66"/>
-      <c r="J32" s="66"/>
-      <c r="K32" s="66"/>
-      <c r="L32" s="66"/>
-      <c r="M32" s="66"/>
-      <c r="N32" s="66"/>
-      <c r="O32" s="66"/>
-      <c r="P32" s="66"/>
-      <c r="Q32" s="66"/>
-      <c r="R32" s="66"/>
-      <c r="S32" s="66"/>
-      <c r="T32" s="66"/>
-      <c r="U32" s="66"/>
-      <c r="V32" s="66"/>
-      <c r="W32" s="66"/>
-      <c r="X32" s="66"/>
-      <c r="Y32" s="66"/>
-      <c r="Z32" s="66"/>
-      <c r="AA32" s="66"/>
-      <c r="AB32" s="66"/>
-      <c r="AC32" s="66"/>
-      <c r="AD32" s="66"/>
-      <c r="AE32" s="66"/>
-      <c r="AF32" s="66"/>
-      <c r="AG32" s="66"/>
-      <c r="AH32" s="66"/>
-      <c r="AI32" s="66"/>
-      <c r="AJ32" s="66"/>
-      <c r="AK32" s="66"/>
-      <c r="AL32" s="66"/>
-      <c r="AM32" s="66"/>
-      <c r="AN32" s="66"/>
-      <c r="AO32" s="66"/>
-      <c r="AP32" s="66"/>
-      <c r="AQ32" s="66"/>
-      <c r="AR32" s="66"/>
-      <c r="AS32" s="66"/>
-      <c r="AT32" s="66"/>
-      <c r="AU32" s="66"/>
-      <c r="AV32" s="66"/>
-      <c r="AW32" s="66"/>
-      <c r="AX32" s="66"/>
-      <c r="AY32" s="66"/>
-      <c r="AZ32" s="66"/>
-      <c r="BA32" s="66"/>
-      <c r="BB32" s="66"/>
-      <c r="BC32" s="66"/>
-      <c r="BD32" s="66"/>
-      <c r="BE32" s="66"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="6"/>
-      <c r="G33" s="6"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="F34" s="77">
+      <c r="I32" s="64"/>
+      <c r="J32" s="64"/>
+      <c r="K32" s="64"/>
+      <c r="L32" s="64"/>
+      <c r="M32" s="64"/>
+      <c r="N32" s="64"/>
+      <c r="O32" s="64"/>
+      <c r="P32" s="64"/>
+      <c r="Q32" s="64"/>
+      <c r="R32" s="64"/>
+      <c r="S32" s="64"/>
+      <c r="T32" s="64"/>
+      <c r="U32" s="64"/>
+      <c r="V32" s="64"/>
+      <c r="W32" s="64"/>
+      <c r="X32" s="64"/>
+      <c r="Y32" s="64"/>
+      <c r="Z32" s="64"/>
+      <c r="AA32" s="64"/>
+      <c r="AB32" s="64"/>
+      <c r="AC32" s="64"/>
+      <c r="AD32" s="64"/>
+      <c r="AE32" s="83"/>
+      <c r="AF32" s="64"/>
+      <c r="AG32" s="64"/>
+      <c r="AH32" s="64"/>
+      <c r="AI32" s="64"/>
+      <c r="AJ32" s="64"/>
+      <c r="AK32" s="64"/>
+      <c r="AL32" s="64"/>
+      <c r="AM32" s="64"/>
+      <c r="AN32" s="64"/>
+      <c r="AO32" s="64"/>
+      <c r="AP32" s="64"/>
+      <c r="AQ32" s="85"/>
+      <c r="AR32" s="64"/>
+      <c r="AS32" s="64"/>
+      <c r="AT32" s="64"/>
+      <c r="AU32" s="64"/>
+      <c r="AV32" s="64"/>
+      <c r="AW32" s="64"/>
+      <c r="AX32" s="84"/>
+      <c r="AY32" s="64"/>
+      <c r="AZ32" s="64"/>
+      <c r="BA32" s="64"/>
+      <c r="BB32" s="64"/>
+      <c r="BC32" s="64"/>
+      <c r="BD32" s="64"/>
+      <c r="BE32" s="64"/>
+    </row>
+    <row r="33" spans="1:57" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="19"/>
+      <c r="B33" s="58"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="62"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="63" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="I33" s="66"/>
+      <c r="J33" s="66"/>
+      <c r="K33" s="66"/>
+      <c r="L33" s="66"/>
+      <c r="M33" s="66"/>
+      <c r="N33" s="66"/>
+      <c r="O33" s="66"/>
+      <c r="P33" s="66"/>
+      <c r="Q33" s="66"/>
+      <c r="R33" s="66"/>
+      <c r="S33" s="66"/>
+      <c r="T33" s="66"/>
+      <c r="U33" s="66"/>
+      <c r="V33" s="66"/>
+      <c r="W33" s="66"/>
+      <c r="X33" s="66"/>
+      <c r="Y33" s="66"/>
+      <c r="Z33" s="66"/>
+      <c r="AA33" s="66"/>
+      <c r="AB33" s="66"/>
+      <c r="AC33" s="66"/>
+      <c r="AD33" s="66"/>
+      <c r="AE33" s="66"/>
+      <c r="AF33" s="66"/>
+      <c r="AG33" s="66"/>
+      <c r="AH33" s="66"/>
+      <c r="AI33" s="66"/>
+      <c r="AJ33" s="66"/>
+      <c r="AK33" s="66"/>
+      <c r="AL33" s="66"/>
+      <c r="AM33" s="66"/>
+      <c r="AN33" s="66"/>
+      <c r="AO33" s="66"/>
+      <c r="AP33" s="66"/>
+      <c r="AQ33" s="66"/>
+      <c r="AR33" s="66"/>
+      <c r="AS33" s="66"/>
+      <c r="AT33" s="66"/>
+      <c r="AU33" s="66"/>
+      <c r="AV33" s="66"/>
+      <c r="AW33" s="66"/>
+      <c r="AX33" s="66"/>
+      <c r="AY33" s="66"/>
+      <c r="AZ33" s="66"/>
+      <c r="BA33" s="66"/>
+      <c r="BB33" s="66"/>
+      <c r="BC33" s="66"/>
+      <c r="BD33" s="66"/>
+      <c r="BE33" s="66"/>
+    </row>
+    <row r="34" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="G34" s="6"/>
+    </row>
+    <row r="35" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="F35" s="77">
         <v>43113</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B35" s="81"/>
-      <c r="C35" s="18"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B36" s="80"/>
+    <row r="36" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="B36" s="81"/>
+      <c r="C36" s="18"/>
+    </row>
+    <row r="37" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="B37" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E14:F14"/>
     <mergeCell ref="J1:AA1"/>
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
@@ -3915,14 +4002,8 @@
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E14:F14"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D32">
+  <conditionalFormatting sqref="D7:D33">
     <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -3936,12 +4017,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BE32">
+  <conditionalFormatting sqref="I5:BE33">
     <cfRule type="expression" dxfId="2" priority="27">
       <formula>AND(today&gt;=I$5,today&lt;I$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BE32">
+  <conditionalFormatting sqref="I7:BE33">
     <cfRule type="expression" dxfId="1" priority="25">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -3974,7 +4055,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D32</xm:sqref>
+          <xm:sqref>D7:D33</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3988,103 +4069,103 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="87.1796875" style="67" customWidth="1"/>
-    <col min="3" max="16384" width="9.1796875" style="2"/>
+    <col min="1" max="1" width="2.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="87.140625" style="67" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:3" s="69" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:3" s="69" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="68" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="68"/>
     </row>
-    <row r="3" spans="2:3" s="71" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:3" s="71" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="70" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="70"/>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="79" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="2:3" s="72" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:3" s="72" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B6" s="74" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="58" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" ht="60" x14ac:dyDescent="0.2">
       <c r="B7" s="75" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" ht="15" x14ac:dyDescent="0.2">
       <c r="B8" s="73"/>
     </row>
-    <row r="9" spans="2:3" s="72" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+    <row r="9" spans="2:3" s="72" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B9" s="74" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="58" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" ht="60" x14ac:dyDescent="0.2">
       <c r="B10" s="75" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="14" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B11" s="76" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" ht="15" x14ac:dyDescent="0.2">
       <c r="B12" s="73"/>
     </row>
-    <row r="13" spans="2:3" ht="14" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B13" s="82" t="str">
         <f>HYPERLINK("https://vertex42.link/HowToMakeAGanttChart","► Watch How This Gantt Chart Was Created")</f>
         <v>► Watch How This Gantt Chart Was Created</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" ht="15" x14ac:dyDescent="0.2">
       <c r="B14" s="73"/>
     </row>
-    <row r="15" spans="2:3" s="72" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+    <row r="15" spans="2:3" s="72" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B15" s="74" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="29" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3" ht="30" x14ac:dyDescent="0.2">
       <c r="B16" s="75" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B17" s="76" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" ht="15" x14ac:dyDescent="0.2">
       <c r="B18" s="73"/>
     </row>
-    <row r="19" spans="2:2" s="72" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+    <row r="19" spans="2:2" s="72" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B19" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="58" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" ht="60" x14ac:dyDescent="0.2">
       <c r="B20" s="75" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" ht="15" x14ac:dyDescent="0.2">
       <c r="B21" s="73"/>
     </row>
-    <row r="22" spans="2:2" ht="72.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" ht="75" x14ac:dyDescent="0.2">
       <c r="B22" s="75" t="s">
         <v>15</v>
       </c>

</xml_diff>